<commit_message>
Preliminary changes for open-day
- Many cosmetic changes
- Implementation of Aggregation functionality for historic Queries
</commit_message>
<xml_diff>
--- a/Captured data/Latency test.xlsx
+++ b/Captured data/Latency test.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -89,10 +89,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,7 +397,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,22 +408,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -436,6 +436,10 @@
       </c>
       <c r="C3">
         <v>0.61770000000000003</v>
+      </c>
+      <c r="D3">
+        <f>SUM(A3:C3)</f>
+        <v>17.523299999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>